<commit_message>
updated fault injection excel sheet
</commit_message>
<xml_diff>
--- a/FPGA_faults_and_sizes.xlsx
+++ b/FPGA_faults_and_sizes.xlsx
@@ -1,20 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitch\Documents\github_repos\ECE2165\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mitch/Documents/dca/ECE2165-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EE6493-07E1-E04C-A2CC-31DBA89039A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet2!$E$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet2!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet2!$F$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet2!$F$2:$F$12</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet2!$G$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet2!$G$2:$G$12</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet2!$D$2:$D$12</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet2!$D$1</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet2!$D$2:$D$12</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet2!$E$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet2!$E$2:$E$12</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Sheet2!$F$1</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Sheet2!$F$2:$F$12</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Sheet2!$G$1</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Sheet2!$G$2:$G$12</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>Zscore</t>
   </si>
@@ -58,11 +78,26 @@
   <si>
     <t>Bit flips in FPGA configuration</t>
   </si>
+  <si>
+    <t>Percentage utilization</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Rzscore</t>
+  </si>
+  <si>
+    <t>Rcusum</t>
+  </si>
+  <si>
+    <t>Rderiv</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,10 +129,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,7 +190,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -252,7 +286,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -517,7 +550,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -618,7 +650,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -735,7 +766,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -852,7 +882,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1036,7 +1065,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1143,7 +1171,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1244,7 +1271,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1362,7 +1388,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1480,7 +1505,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1664,7 +1688,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1771,7 +1794,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1872,7 +1894,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1998,7 +2019,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2124,7 +2144,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2316,7 +2335,743 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Reliability</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Vs Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rzscore</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99012676579762737</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98119313121828544</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97310967799907222</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.965795497486439</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95917738080776183</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95318908611132447</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94777067554039651</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.94286791530506442</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93843173284703452</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.93441772566407888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-58F5-6147-9DC7-520C42CE6F4C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rcusum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99799273416947787</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99617649249365747</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99453309590172301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99304609535860289</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99170060722379039</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99048316427846184</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98938158092980089</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98838483124333443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98748293858248526</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98666687575072531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-58F5-6147-9DC7-520C42CE6F4C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rderiv</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99885957875009224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9978276872235301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99689399704310155</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99604916274551514</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99528472824107295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99459304217523592</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9939671813449189</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99340088140297766</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99288847415729631</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99242483083689115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-58F5-6147-9DC7-520C42CE6F4C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1981657391"/>
+        <c:axId val="1981671839"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1981657391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (years)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1981671839"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1981671839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.92"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Reliability</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1981657391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2543,6 +3298,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4202,6 +4997,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4572,7 +5883,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4602,7 +5919,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4632,7 +5955,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4662,7 +5991,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4672,6 +6007,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DBD7F32-A257-A843-BB90-28FE3D60095A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4942,31 +6318,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4974,7 +6350,7 @@
         <v>1.3103</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4982,7 +6358,7 @@
         <v>9.7032000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4990,66 +6366,66 @@
         <v>1.1482000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+    <row r="33" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+    <row r="34" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
     </row>
-    <row r="40" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="1" t="s">
+    <row r="40" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="J40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="K41" s="2" t="s">
+    <row r="41" spans="9:15" x14ac:dyDescent="0.2">
+      <c r="K41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="L41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M41" s="2"/>
+      <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="9:15" x14ac:dyDescent="0.2">
       <c r="J42" t="s">
         <v>0</v>
       </c>
@@ -5059,8 +6435,15 @@
       <c r="L42">
         <v>448</v>
       </c>
+      <c r="N42">
+        <f>K42/O42</f>
+        <v>0.13593984962406014</v>
+      </c>
+      <c r="O42">
+        <v>13300</v>
+      </c>
     </row>
-    <row r="43" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="9:15" x14ac:dyDescent="0.2">
       <c r="J43" t="s">
         <v>1</v>
       </c>
@@ -5070,8 +6453,12 @@
       <c r="L43">
         <v>768</v>
       </c>
+      <c r="N43">
+        <f>K43/O42</f>
+        <v>0.20466165413533835</v>
+      </c>
     </row>
-    <row r="44" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="9:15" x14ac:dyDescent="0.2">
       <c r="J44" t="s">
         <v>2</v>
       </c>
@@ -5081,23 +6468,27 @@
       <c r="L44">
         <v>160</v>
       </c>
+      <c r="N44">
+        <f>K44/O42</f>
+        <v>1.3759398496240602E-2</v>
+      </c>
     </row>
-    <row r="49" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="J49" s="1" t="s">
+    <row r="49" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="K50" s="2" t="s">
+    <row r="50" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="K50" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L50" s="2" t="s">
+      <c r="L50" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="10:20" x14ac:dyDescent="0.2">
       <c r="J51" t="s">
         <v>0</v>
       </c>
@@ -5110,7 +6501,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="52" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="10:20" x14ac:dyDescent="0.2">
       <c r="J52" t="s">
         <v>1</v>
       </c>
@@ -5123,7 +6514,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="53" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="10:20" x14ac:dyDescent="0.2">
       <c r="J53" t="s">
         <v>2</v>
       </c>
@@ -5136,22 +6527,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="R56" s="1" t="s">
+    <row r="56" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="R56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
     </row>
-    <row r="57" spans="10:20" x14ac:dyDescent="0.25">
-      <c r="S57" s="2" t="s">
+    <row r="57" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="S57" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="T57" s="2" t="s">
+      <c r="T57" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="10:20" x14ac:dyDescent="0.2">
       <c r="R58" t="s">
         <v>0</v>
       </c>
@@ -5164,7 +6555,7 @@
         <v>2.9247767857142857</v>
       </c>
     </row>
-    <row r="59" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="10:20" x14ac:dyDescent="0.2">
       <c r="R59" t="s">
         <v>1</v>
       </c>
@@ -5177,7 +6568,7 @@
         <v>12.634375000000002</v>
       </c>
     </row>
-    <row r="60" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="10:20" x14ac:dyDescent="0.2">
       <c r="R60" t="s">
         <v>2</v>
       </c>
@@ -5200,4 +6591,260 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379FEB30-4584-C04E-BFB1-1C901D179617}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.13593984962406014</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>1-((1-EXP(-11416/1000000000*8760*D2))*$B$2/$B$8)</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>1-((1-EXP(-11416/1000000000*8760*D2))*$B$3/$B$9)</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f>1-((1-EXP(-11416/1000000000*8760*D2))*$B$4/$B$10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.20466165413533835</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E52" si="0">1-((1-EXP(-11416/1000000000*8760*D3))*$B$2/$B$8)</f>
+        <v>0.99012676579762737</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F52" si="1">1-((1-EXP(-11416/1000000000*8760*D3))*$B$3/$B$9)</f>
+        <v>0.99799273416947787</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G52" si="2">1-((1-EXP(-11416/1000000000*8760*D3))*$B$4/$B$10)</f>
+        <v>0.99885957875009224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1.3759398496240602E-2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.98119313121828544</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>0.99617649249365747</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0.9978276872235301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.97310967799907222</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.99453309590172301</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0.99689399704310155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.965795497486439</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.99304609535860289</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0.99604916274551514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.95917738080776183</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.99170060722379039</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0.99528472824107295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1.3103</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.95318908611132447</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0.99048316427846184</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0.99459304217523592</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>9.7032000000000007</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.94777067554039651</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.98938158092980089</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0.9939671813449189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1.1482000000000001</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.94286791530506442</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.98838483124333443</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.99340088140297766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.93843173284703452</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.98748293858248526</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0.99288847415729631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.93441772566407888</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.98666687575072531</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0.99242483083689115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>